<commit_message>
added and updated a notes markdown file
</commit_message>
<xml_diff>
--- a/Excel101ExtraPractice-01.xlsx
+++ b/Excel101ExtraPractice-01.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://weifieldgroup0-my.sharepoint.com/personal/cjones_weifieldgroup_com/Documents/Desktop/Excel_Udemy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7D71B455-60BB-4BCF-AAB8-54DBE784D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B7AA266-B10A-437B-B3B3-4097048BB08E}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{7D71B455-60BB-4BCF-AAB8-54DBE784D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{389519B9-C0A5-4AEA-98D4-9D4494F50755}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7A83C70D-7383-4E55-840F-4FA78D0040E1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{7A83C70D-7383-4E55-840F-4FA78D0040E1}"/>
   </bookViews>
   <sheets>
     <sheet name="EXCEL 101 PRACTICE" sheetId="4" r:id="rId1"/>
     <sheet name="Formatting Spread Sheet" sheetId="1" r:id="rId2"/>
-    <sheet name="Column Chart" sheetId="2" r:id="rId3"/>
-    <sheet name="Template" sheetId="3" r:id="rId4"/>
+    <sheet name="Sales_report" sheetId="5" r:id="rId3"/>
+    <sheet name="Column Chart" sheetId="2" r:id="rId4"/>
+    <sheet name="Template" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Orders">#REF!</definedName>
@@ -539,12 +540,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="6" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -564,10 +562,13 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -777,7 +778,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F121-4A7D-886E-E5AB5BDFB90E}"/>
+              <c16:uniqueId val="{00000000-9C4D-41C1-A364-7FB57021CB7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -877,7 +878,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F121-4A7D-886E-E5AB5BDFB90E}"/>
+              <c16:uniqueId val="{00000001-9C4D-41C1-A364-7FB57021CB7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -977,7 +978,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F121-4A7D-886E-E5AB5BDFB90E}"/>
+              <c16:uniqueId val="{00000002-9C4D-41C1-A364-7FB57021CB7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1077,7 +1078,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F121-4A7D-886E-E5AB5BDFB90E}"/>
+              <c16:uniqueId val="{00000003-9C4D-41C1-A364-7FB57021CB7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1284,11 +1285,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1402,6 +1398,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-60BC-48C4-B489-9AAB4B4B9114}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1444,6 +1445,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-60BC-48C4-B489-9AAB4B4B9114}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1486,6 +1492,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-60BC-48C4-B489-9AAB4B4B9114}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1528,6 +1539,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-60BC-48C4-B489-9AAB4B4B9114}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2804,6 +2820,17 @@
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AB4B1347-72BC-46FD-BF2C-E8A7A09A1BEC}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3626,6 +3653,39 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8668058" cy="6288350"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5022CCE-F924-848D-3052-6CB251DDA9E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -3854,42 +3914,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>387568</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>89994</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>72258</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>120211</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3F20713-48ED-D86A-3E88-D93FDB406E75}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>354724</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -3918,7 +3942,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3927,7 +3951,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4044,6 +4068,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4347,7 +4375,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4362,19 +4390,19 @@
       <selection activeCell="B4" sqref="B4:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="24.5" x14ac:dyDescent="1.1499999999999999"/>
   <cols>
-    <col min="1" max="1" width="18" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="18" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="B1" s="48" t="s">
         <v>15</v>
       </c>
@@ -4385,7 +4413,7 @@
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
     </row>
-    <row r="2" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:8" ht="25" thickBot="1" x14ac:dyDescent="1.2">
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
@@ -4394,218 +4422,218 @@
       <c r="G2" s="48"/>
       <c r="H2" s="48"/>
     </row>
-    <row r="3" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:8" ht="25" thickBot="1" x14ac:dyDescent="1.2">
+      <c r="A3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.8">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="1.1499999999999999">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="26">
         <v>2500</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>3075</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <v>1850</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <v>3500</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="27">
         <f>SUM(B4:E4)</f>
         <v>10925</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="32">
         <f>F4/$F$8</f>
         <v>0.249002849002849</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.8">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="1.1499999999999999">
+      <c r="A5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="26">
         <v>3025</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>3500</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <v>2500</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <v>1650</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <f t="shared" ref="F5:F7" si="0">SUM(B5:E5)</f>
         <v>10675</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="32">
         <f t="shared" ref="G5:G8" si="1">F5/$F$8</f>
         <v>0.24330484330484331</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.8">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="1.1499999999999999">
+      <c r="A6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="26">
         <v>1750</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>3750</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <v>2750</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <v>4000</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <f t="shared" si="0"/>
         <v>12250</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="32">
         <f t="shared" si="1"/>
         <v>0.27920227920227919</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.8">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="1.1499999999999999">
+      <c r="A7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
         <v>3500</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>2000</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <v>1500</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>3025</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <f t="shared" si="0"/>
         <v>10025</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="32">
         <f t="shared" si="1"/>
         <v>0.2284900284900285</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:8" ht="25" thickBot="1" x14ac:dyDescent="1.2">
+      <c r="A8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="28">
         <f>SUM(B4:B7)</f>
         <v>10775</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <f t="shared" ref="C8:E8" si="2">SUM(C4:C7)</f>
         <v>12325</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <f t="shared" si="2"/>
         <v>8600</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <f t="shared" si="2"/>
         <v>12175</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <f>SUM(B8:E8)</f>
         <v>43875</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.85"/>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.8">
-      <c r="A10" s="45" t="s">
+    <row r="9" spans="1:8" ht="25" thickBot="1" x14ac:dyDescent="1.2"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="1.1499999999999999">
+      <c r="A10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="37">
         <f>AVERAGE(B4:B7)</f>
         <v>2693.75</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="38">
         <f t="shared" ref="C10:E10" si="3">AVERAGE(C4:C7)</f>
         <v>3081.25</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="38">
         <f t="shared" si="3"/>
         <v>2150</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <f t="shared" si="3"/>
         <v>3043.75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.8">
-      <c r="A11" s="46" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="1.1499999999999999">
+      <c r="A11" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="40">
         <f>MIN(B4:B7)</f>
         <v>1750</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="27">
         <f t="shared" ref="C11:E11" si="4">MIN(C4:C7)</f>
         <v>2000</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <f t="shared" si="4"/>
         <v>1500</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="41">
         <f t="shared" si="4"/>
         <v>1650</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="A12" s="47" t="s">
+    <row r="12" spans="1:8" ht="25" thickBot="1" x14ac:dyDescent="1.2">
+      <c r="A12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="42">
         <f>MAX(B4:B7)</f>
         <v>3500</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <f t="shared" ref="C12:E12" si="5">MAX(C4:C7)</f>
         <v>3750</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <f t="shared" si="5"/>
         <v>2750</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="43">
         <f t="shared" si="5"/>
         <v>4000</v>
       </c>
@@ -4627,25 +4655,25 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4662,7 +4690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -4679,7 +4707,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -4696,7 +4724,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -4713,7 +4741,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -4743,32 +4771,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A91FA97-13A8-46BA-97F2-B1567C89A7AC}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>0</v>
       </c>
@@ -4792,20 +4820,20 @@
       </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="47">
         <v>2500</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="47">
         <v>3075</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="47">
         <v>1850</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="47">
         <v>3500</v>
       </c>
       <c r="F9" s="16">
@@ -4817,20 +4845,20 @@
         <v>0.249002849002849</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="47">
         <v>3025</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="47">
         <v>3500</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="47">
         <v>2500</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="47">
         <v>1650</v>
       </c>
       <c r="F10" s="16">
@@ -4842,20 +4870,20 @@
         <v>0.24330484330484331</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="47">
         <v>1750</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="47">
         <v>3750</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="47">
         <v>2750</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="47">
         <v>4000</v>
       </c>
       <c r="F11" s="16">
@@ -4867,20 +4895,20 @@
         <v>0.27920227920227919</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="47">
         <v>3500</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="47">
         <v>2000</v>
       </c>
-      <c r="D12" s="49">
+      <c r="D12" s="47">
         <v>1500</v>
       </c>
-      <c r="E12" s="49">
+      <c r="E12" s="47">
         <v>3025</v>
       </c>
       <c r="F12" s="16">
@@ -4892,7 +4920,7 @@
         <v>0.2284900284900285</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -4913,7 +4941,7 @@
         <v>12175</v>
       </c>
       <c r="F13" s="17">
-        <f t="shared" ref="F10:F13" si="3">SUM(B13:E13)</f>
+        <f t="shared" ref="F13" si="3">SUM(B13:E13)</f>
         <v>43875</v>
       </c>
       <c r="G13" s="19">
@@ -4921,8 +4949,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -4951,7 +4979,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -4980,7 +5008,7 @@
         <v>0.2284900284900285</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>

</xml_diff>